<commit_message>
fixed typo in Olker supp table and add filtering step for mc6 flags altho it doesn't change priority chems
</commit_message>
<xml_diff>
--- a/data/olker19_assay_interference_suppTable5.xlsx
+++ b/data/olker19_assay_interference_suppTable5.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktruong\thyroid_prioritization\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/truong_kimberly_epa_gov/Documents/Profile/Documents/CompTox-thyroid-httk/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41402F96-3CC7-44E4-9501-9A1DDDB70467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{41402F96-3CC7-44E4-9501-9A1DDDB70467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5287EA1-941F-4181-9190-249515E1A842}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E90EEA9F-BF31-4B4B-8EAE-42E1407E01C7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E90EEA9F-BF31-4B4B-8EAE-42E1407E01C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$33</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -72,9 +75,6 @@
     <t>83657-24-3</t>
   </si>
   <si>
-    <t>Abnormal time course of absorbance at 420 nmb</t>
-  </si>
-  <si>
     <t>9-Phenanthrol</t>
   </si>
   <si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>5700-49-2</t>
+  </si>
+  <si>
+    <t>Abnormal time course of absorbance at 420 nm</t>
   </si>
 </sst>
 </file>
@@ -314,10 +317,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -355,7 +362,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -461,7 +468,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -603,7 +610,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -614,7 +621,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -672,32 +679,32 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -705,139 +712,139 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1">
         <v>1823692</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
         <v>35</v>
       </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
       <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
         <v>37</v>
-      </c>
-      <c r="D15" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
         <v>39</v>
       </c>
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -845,13 +852,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
         <v>41</v>
       </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -859,13 +866,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
         <v>43</v>
       </c>
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -873,13 +880,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
         <v>45</v>
       </c>
-      <c r="B19" t="s">
-        <v>46</v>
-      </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -887,201 +894,202 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
         <v>47</v>
       </c>
-      <c r="B20" t="s">
-        <v>48</v>
-      </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
         <v>49</v>
       </c>
-      <c r="B21" t="s">
-        <v>50</v>
-      </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
         <v>51</v>
       </c>
-      <c r="B22" t="s">
-        <v>52</v>
-      </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
         <v>53</v>
       </c>
-      <c r="B23" t="s">
-        <v>54</v>
-      </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
         <v>55</v>
       </c>
-      <c r="B24" t="s">
-        <v>56</v>
-      </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
         <v>57</v>
       </c>
-      <c r="B25" t="s">
-        <v>58</v>
-      </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
         <v>59</v>
       </c>
-      <c r="B26" t="s">
-        <v>60</v>
-      </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
         <v>61</v>
       </c>
-      <c r="B27" t="s">
-        <v>62</v>
-      </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" t="s">
         <v>63</v>
       </c>
-      <c r="B28" t="s">
-        <v>64</v>
-      </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
         <v>65</v>
       </c>
-      <c r="B29" t="s">
-        <v>66</v>
-      </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" t="s">
         <v>67</v>
       </c>
-      <c r="B30" t="s">
-        <v>68</v>
-      </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" t="s">
         <v>69</v>
       </c>
-      <c r="B31" t="s">
-        <v>70</v>
-      </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s">
         <v>71</v>
       </c>
-      <c r="B32" t="s">
-        <v>72</v>
-      </c>
       <c r="C32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" t="s">
         <v>73</v>
       </c>
-      <c r="B33" t="s">
-        <v>74</v>
-      </c>
       <c r="C33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D33" xr:uid="{88DF7FCA-EEC3-4EBB-AA52-EF9713C8F9AF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>